<commit_message>
added the tables data
</commit_message>
<xml_diff>
--- a/05_Snowflake_Advance_DE_Certificate/Domain_Wise_Flow_Lost.xlsx
+++ b/05_Snowflake_Advance_DE_Certificate/Domain_Wise_Flow_Lost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Snowflake_Advance_Data_Engineering\05_Snowflake_Advance_DE_Certificate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A84E9-875D-407C-A76A-875544AA8A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14689AB-923A-4073-B501-7E9CFA7E32CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1383,6 +1383,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1397,12 +1403,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1689,20 +1689,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="83" workbookViewId="0">
-      <selection activeCell="M18" sqref="I18:M18"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="102" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
@@ -1721,7 +1735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="57.6">
+    <row r="3" spans="1:13" ht="43.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="72">
+    <row r="4" spans="1:13" ht="43.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1755,7 +1769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="72">
+    <row r="5" spans="1:13" ht="56.4">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1803,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="43.2">
+    <row r="7" spans="1:13" ht="28.8">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1840,7 +1854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="57.6">
+    <row r="10" spans="1:13" ht="43.2">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -1867,16 +1881,16 @@
       <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="E16" s="8" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="E16" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -1953,7 +1967,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.2">
+    <row r="19" spans="1:13" ht="28.8">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
         <v>47</v>
@@ -2388,7 +2402,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="28.8">
+    <row r="32" spans="1:13">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
         <v>60</v>
@@ -2424,7 +2438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="28.8">
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>1.5</v>
       </c>
@@ -2592,7 +2606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.8">
+    <row r="43" spans="1:7">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
         <v>71</v>
@@ -2628,7 +2642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8">
+    <row r="45" spans="1:7">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
         <v>73</v>
@@ -2646,7 +2660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="28.8">
+    <row r="46" spans="1:7">
       <c r="A46" s="3"/>
       <c r="B46" s="4" t="s">
         <v>74</v>
@@ -2814,7 +2828,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="28.8">
+    <row r="56" spans="1:7">
       <c r="E56" s="3">
         <v>39</v>
       </c>
@@ -2858,7 +2872,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.8">
+    <row r="60" spans="1:7">
       <c r="E60" s="3">
         <v>43</v>
       </c>
@@ -2869,7 +2883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28.8">
+    <row r="61" spans="1:7">
       <c r="E61" s="3">
         <v>44</v>
       </c>
@@ -2914,35 +2928,35 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2963,7 +2977,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="43.2">
+    <row r="73" spans="1:5" ht="28.8">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
@@ -3208,13 +3222,13 @@
   <sheetFormatPr defaultColWidth="35.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
@@ -3370,16 +3384,16 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="E16" s="8" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="E16" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">

</xml_diff>